<commit_message>
Correction cardinalité PR.name.prefix a27f50f2a964294bb099df6f48cdd62322ed624d
</commit_message>
<xml_diff>
--- a/ig/295-erreur-cardinalite-practitionner-civilité/StructureDefinition-ror-practitioner.xlsx
+++ b/ig/295-erreur-cardinalite-practitionner-civilité/StructureDefinition-ror-practitioner.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-26T15:22:17+00:00</t>
+    <t>2024-01-26T15:42:02+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -6197,7 +6197,7 @@
         <v>77</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>76</v>

</xml_diff>